<commit_message>
added manual review data to fastqfile sheets
</commit_message>
<xml_diff>
--- a/fastqFiles/fastqFiles_01.13.20.xlsx
+++ b/fastqFiles/fastqFiles_01.13.20.xlsx
@@ -233,13 +233,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,17 +260,10 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Menlo"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -283,12 +275,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -317,25 +316,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -347,66 +334,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF222222"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -415,51 +342,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y53"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="L:P"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="85.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1"/>
@@ -467,21 +392,12 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -493,7 +409,7 @@
       <c r="E2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -502,35 +418,21 @@
       <c r="H2" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="0" t="n">
         <v>0.967550218694314</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>7398727</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -542,7 +444,7 @@
       <c r="E3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -551,21 +453,21 @@
       <c r="H3" s="0" t="n">
         <v>49.2</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="0" t="n">
         <v>0.97852754454229</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>7738807</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -577,7 +479,7 @@
       <c r="E4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -586,21 +488,21 @@
       <c r="H4" s="0" t="n">
         <v>11.1</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="0" t="n">
         <v>0.835224094532233</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>7791399</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -612,7 +514,7 @@
       <c r="E5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -621,21 +523,21 @@
       <c r="H5" s="0" t="n">
         <v>1.98</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="0" t="n">
         <v>4.33650656653735</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>7513811</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -647,7 +549,7 @@
       <c r="E6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -656,21 +558,21 @@
       <c r="H6" s="0" t="n">
         <v>6.96</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="0" t="n">
         <v>1.46260131364289</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>7209266</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -682,7 +584,7 @@
       <c r="E7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -691,21 +593,21 @@
       <c r="H7" s="0" t="n">
         <v>44.8</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="0" t="n">
         <v>0.972869242985707</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>7557400</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -717,7 +619,7 @@
       <c r="E8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="0" t="s">
@@ -726,21 +628,21 @@
       <c r="H8" s="0" t="n">
         <v>0.256</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="0" t="n">
         <v>6.56122981434692</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>5700146</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -752,7 +654,7 @@
       <c r="E9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="0" t="s">
@@ -761,21 +663,21 @@
       <c r="H9" s="0" t="n">
         <v>27.5</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="0" t="n">
         <v>1.31145358730856</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>6563888</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -787,7 +689,7 @@
       <c r="E10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -796,21 +698,21 @@
       <c r="H10" s="0" t="n">
         <v>50.3</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="0" t="n">
         <v>0.94358979422568</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>387536</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -822,7 +724,7 @@
       <c r="E11" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="0" t="s">
@@ -831,21 +733,21 @@
       <c r="H11" s="0" t="n">
         <v>32.1</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="0" t="n">
         <v>1.23383514951196</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>7407190</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -857,7 +759,7 @@
       <c r="E12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="0" t="s">
@@ -866,21 +768,21 @@
       <c r="H12" s="0" t="n">
         <v>12.1</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="0" t="n">
         <v>0.127314124016797</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>33180360</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -892,7 +794,7 @@
       <c r="E13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="0" t="s">
@@ -901,21 +803,21 @@
       <c r="H13" s="0" t="n">
         <v>76.5</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="0" t="n">
         <v>1.04317308532006</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>7363681</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -927,7 +829,7 @@
       <c r="E14" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="0" t="s">
@@ -936,21 +838,21 @@
       <c r="H14" s="0" t="n">
         <v>132</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="0" t="n">
         <v>1.18276894895787</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>7167960</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -962,7 +864,7 @@
       <c r="E15" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="0" t="s">
@@ -971,21 +873,21 @@
       <c r="H15" s="0" t="n">
         <v>29.1</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="0" t="n">
         <v>1.15470033832769</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>8133612</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -997,7 +899,7 @@
       <c r="E16" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="0" t="s">
@@ -1006,21 +908,21 @@
       <c r="H16" s="0" t="n">
         <v>90.4</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="0" t="n">
         <v>1.19001544132297</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>7562359</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -1032,7 +934,7 @@
       <c r="E17" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="0" t="s">
@@ -1041,21 +943,21 @@
       <c r="H17" s="0" t="n">
         <v>37.6</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="0" t="n">
         <v>1.28811937240524</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>7929803</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="0" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -1067,7 +969,7 @@
       <c r="E18" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="0" t="s">
@@ -1076,21 +978,21 @@
       <c r="H18" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="0" t="n">
         <v>1.16500463256449</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>6362673</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -1102,7 +1004,7 @@
       <c r="E19" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="0" t="s">
@@ -1111,21 +1013,21 @@
       <c r="H19" s="0" t="n">
         <v>69.5</v>
       </c>
-      <c r="I19" s="3" t="n">
+      <c r="I19" s="0" t="n">
         <v>1.39900158107396</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>6995825</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -1137,7 +1039,7 @@
       <c r="E20" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="0" t="s">
@@ -1146,21 +1048,21 @@
       <c r="H20" s="0" t="n">
         <v>81.4</v>
       </c>
-      <c r="I20" s="3" t="n">
+      <c r="I20" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>46957365</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -1172,7 +1074,7 @@
       <c r="E21" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="0" t="s">
@@ -1181,21 +1083,21 @@
       <c r="H21" s="0" t="n">
         <v>106</v>
       </c>
-      <c r="I21" s="3" t="n">
+      <c r="I21" s="0" t="n">
         <v>1.0482077044577</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>7695611</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -1207,7 +1109,7 @@
       <c r="E22" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="0" t="s">
@@ -1216,21 +1118,21 @@
       <c r="H22" s="0" t="n">
         <v>22.8</v>
       </c>
-      <c r="I22" s="3" t="n">
+      <c r="I22" s="0" t="n">
         <v>1.30514886642994</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>7669183</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -1242,7 +1144,7 @@
       <c r="E23" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="0" t="s">
@@ -1251,21 +1153,21 @@
       <c r="H23" s="0" t="n">
         <v>2.46</v>
       </c>
-      <c r="I23" s="3" t="n">
+      <c r="I23" s="0" t="n">
         <v>11.7703151034662</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>9219705</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -1277,7 +1179,7 @@
       <c r="E24" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="0" t="s">
@@ -1286,21 +1188,21 @@
       <c r="H24" s="0" t="n">
         <v>48.9</v>
       </c>
-      <c r="I24" s="3" t="n">
+      <c r="I24" s="0" t="n">
         <v>1.19549389511609</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>7057920</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -1312,7 +1214,7 @@
       <c r="E25" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="0" t="s">
@@ -1321,21 +1223,21 @@
       <c r="H25" s="0" t="n">
         <v>0.959</v>
       </c>
-      <c r="I25" s="3" t="n">
+      <c r="I25" s="0" t="n">
         <v>8.87406210534136</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>7028387</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -1347,7 +1249,7 @@
       <c r="E26" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G26" s="0" t="s">
@@ -1356,21 +1258,21 @@
       <c r="H26" s="0" t="n">
         <v>24.9</v>
       </c>
-      <c r="I26" s="3" t="n">
+      <c r="I26" s="0" t="n">
         <v>1.54893348029046</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>6908612</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -1382,7 +1284,7 @@
       <c r="E27" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="0" t="s">
@@ -1391,21 +1293,21 @@
       <c r="H27" s="0" t="n">
         <v>16.6</v>
       </c>
-      <c r="I27" s="3" t="n">
+      <c r="I27" s="0" t="n">
         <v>1.1739349417719</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>6772391</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="0" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="0" t="n">
@@ -1417,7 +1319,7 @@
       <c r="E28" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G28" s="0" t="s">
@@ -1432,15 +1334,15 @@
       <c r="J28" s="0" t="n">
         <v>1168788</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="0" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -1452,7 +1354,7 @@
       <c r="E29" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G29" s="0" t="s">
@@ -1467,16 +1369,15 @@
       <c r="J29" s="0" t="n">
         <v>8305631</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="M29" s="4"/>
-    </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -1488,7 +1389,7 @@
       <c r="E30" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G30" s="0" t="s">
@@ -1503,17 +1404,15 @@
       <c r="J30" s="0" t="n">
         <v>7343496</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M30" s="4"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -1525,7 +1424,7 @@
       <c r="E31" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="0" t="s">
@@ -1540,17 +1439,15 @@
       <c r="J31" s="0" t="n">
         <v>8596343</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="M31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -1562,7 +1459,7 @@
       <c r="E32" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="0" t="s">
@@ -1577,17 +1474,15 @@
       <c r="J32" s="0" t="n">
         <v>7395140</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="M32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="0" t="n">
@@ -1599,7 +1494,7 @@
       <c r="E33" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="0" t="s">
@@ -1614,17 +1509,15 @@
       <c r="J33" s="0" t="n">
         <v>7384004</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="0" t="n">
@@ -1636,7 +1529,7 @@
       <c r="E34" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G34" s="0" t="s">
@@ -1651,17 +1544,15 @@
       <c r="J34" s="0" t="n">
         <v>5367610</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="M34" s="4"/>
-      <c r="O34" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="0" t="n">
@@ -1673,7 +1564,7 @@
       <c r="E35" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="0" t="s">
@@ -1688,17 +1579,15 @@
       <c r="J35" s="0" t="n">
         <v>7112721</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="K35" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="M35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="0" t="n">
@@ -1710,7 +1599,7 @@
       <c r="E36" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="0" t="s">
@@ -1725,17 +1614,15 @@
       <c r="J36" s="0" t="n">
         <v>8763810</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="M36" s="4"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -1747,7 +1634,7 @@
       <c r="E37" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="0" t="s">
@@ -1762,17 +1649,15 @@
       <c r="J37" s="0" t="n">
         <v>9142478</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="M37" s="4"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="0" t="n">
@@ -1784,7 +1669,7 @@
       <c r="E38" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="0" t="s">
@@ -1799,17 +1684,15 @@
       <c r="J38" s="0" t="n">
         <v>9989045</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="K38" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -1821,7 +1704,7 @@
       <c r="E39" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="0" t="s">
@@ -1836,17 +1719,15 @@
       <c r="J39" s="0" t="n">
         <v>7652496</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K39" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="4"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="0" t="n">
@@ -1858,7 +1739,7 @@
       <c r="E40" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="0" t="s">
@@ -1873,17 +1754,15 @@
       <c r="J40" s="0" t="n">
         <v>5989773</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="M40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="0" t="n">
@@ -1895,7 +1774,7 @@
       <c r="E41" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="0" t="s">
@@ -1910,16 +1789,15 @@
       <c r="J41" s="0" t="n">
         <v>7263152</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="M41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="0" t="n">
@@ -1931,7 +1809,7 @@
       <c r="E42" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="0" t="s">
@@ -1946,16 +1824,15 @@
       <c r="J42" s="0" t="n">
         <v>7358865</v>
       </c>
-      <c r="K42" s="4" t="s">
+      <c r="K42" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="0" t="n">
@@ -1967,7 +1844,7 @@
       <c r="E43" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="0" t="s">
@@ -1982,16 +1859,15 @@
       <c r="J43" s="0" t="n">
         <v>7216406</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="0" t="n">
@@ -2003,7 +1879,7 @@
       <c r="E44" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G44" s="0" t="s">
@@ -2018,16 +1894,15 @@
       <c r="J44" s="0" t="n">
         <v>7797092</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K44" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="0" t="n">
@@ -2039,7 +1914,7 @@
       <c r="E45" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G45" s="0" t="s">
@@ -2054,16 +1929,15 @@
       <c r="J45" s="0" t="n">
         <v>7609591</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="M45" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="0" t="n">
@@ -2075,7 +1949,7 @@
       <c r="E46" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G46" s="0" t="s">
@@ -2090,16 +1964,15 @@
       <c r="J46" s="0" t="n">
         <v>6952677</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K46" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="0" t="n">
@@ -2111,7 +1984,7 @@
       <c r="E47" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="0" t="s">
@@ -2126,16 +1999,15 @@
       <c r="J47" s="0" t="n">
         <v>6184498</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="K47" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="M47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="0" t="n">
@@ -2147,7 +2019,7 @@
       <c r="E48" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G48" s="0" t="s">
@@ -2162,16 +2034,15 @@
       <c r="J48" s="0" t="n">
         <v>5170599</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K48" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="M48" s="4"/>
-    </row>
-    <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="0" t="n">
@@ -2183,7 +2054,7 @@
       <c r="E49" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="0" t="s">
@@ -2198,16 +2069,15 @@
       <c r="J49" s="0" t="n">
         <v>4728864</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K49" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M49" s="4"/>
-    </row>
-    <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="0" t="n">
@@ -2219,7 +2089,7 @@
       <c r="E50" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="0" t="s">
@@ -2234,16 +2104,15 @@
       <c r="J50" s="0" t="n">
         <v>5547220</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="M50" s="4"/>
-    </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="0" t="n">
@@ -2255,7 +2124,7 @@
       <c r="E51" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G51" s="0" t="s">
@@ -2270,16 +2139,15 @@
       <c r="J51" s="0" t="n">
         <v>5052913</v>
       </c>
-      <c r="K51" s="4" t="s">
+      <c r="K51" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="M51" s="4"/>
-    </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="0" t="n">
@@ -2291,7 +2159,7 @@
       <c r="E52" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G52" s="0" t="s">
@@ -2306,16 +2174,15 @@
       <c r="J52" s="0" t="n">
         <v>6800026</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="K52" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="M52" s="4"/>
-    </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="0" t="n">
@@ -2327,7 +2194,7 @@
       <c r="E53" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G53" s="0" t="s">
@@ -2342,20 +2209,13 @@
       <c r="J53" s="0" t="n">
         <v>7619975</v>
       </c>
-      <c r="K53" s="4" t="s">
+      <c r="K53" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="M53" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F53" type="list">
-      <formula1>"MidOutput,HighOutput"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>